<commit_message>
copied over latest from private repo
</commit_message>
<xml_diff>
--- a/pathways workbook - ethiopia 2016.xlsx
+++ b/pathways workbook - ethiopia 2016.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://bmgf-my.sharepoint.com/personal/jeremy_cooper_gatesfoundation_org/Documents/scenario_dhs_ethiopia_2016/workshop_prep/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="683" documentId="11_A09B48BC4F10D9CFB369C71317FDCB2BF82E9003" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{ECCB6027-FA62-4571-B6AA-FDD258EB60E6}"/>
+  <xr:revisionPtr revIDLastSave="1002" documentId="11_A09B48BC4F10D9CFB369C71317FDCB2BF82E9003" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{68E16191-16AB-4AE1-BC77-F04912FA747E}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11620" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-11310" yWindow="-21600" windowWidth="25800" windowHeight="21000" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="params" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1191" uniqueCount="996">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1212" uniqueCount="1008">
   <si>
     <t>domains</t>
   </si>
@@ -3008,9 +3008,6 @@
     <t>check</t>
   </si>
   <si>
-    <t>recode</t>
-  </si>
-  <si>
     <t xml:space="preserve">this drops because jd.index.cat is fixed </t>
   </si>
   <si>
@@ -3027,6 +3024,45 @@
   </si>
   <si>
     <t>HH Wboth</t>
+  </si>
+  <si>
+    <t>&lt;18, 18-25, 25+</t>
+  </si>
+  <si>
+    <t>using ed.level</t>
+  </si>
+  <si>
+    <t>collapse not partnered/other</t>
+  </si>
+  <si>
+    <t>combine secondary + higher</t>
+  </si>
+  <si>
+    <t>using polygamy</t>
+  </si>
+  <si>
+    <t>using Y/N variable</t>
+  </si>
+  <si>
+    <t>add HH Sanitation</t>
+  </si>
+  <si>
+    <t>recode (looks good)</t>
+  </si>
+  <si>
+    <t>fix</t>
+  </si>
+  <si>
+    <t>collapse not partnered/other, respondent and huband/partner</t>
+  </si>
+  <si>
+    <t>collapse 0 into 0-1</t>
+  </si>
+  <si>
+    <t>categorical (0, 1-2, 3-4)</t>
+  </si>
+  <si>
+    <t>0, 1-3, 4+</t>
   </si>
 </sst>
 </file>
@@ -3436,7 +3472,7 @@
   <dimension ref="A1:H72"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C42" sqref="C42"/>
+      <selection activeCell="A3" sqref="A3:A72"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4643,8 +4679,8 @@
   <dimension ref="A1:T284"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F24" sqref="A1:T284"/>
+      <pane ySplit="1" topLeftCell="A15" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A162" sqref="A162"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="74" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4662,7 +4698,7 @@
     <col min="11" max="11" width="15.6328125" hidden="1" customWidth="1"/>
     <col min="12" max="12" width="18.36328125" hidden="1" customWidth="1"/>
     <col min="13" max="13" width="19.6328125" hidden="1" customWidth="1"/>
-    <col min="14" max="14" width="13.90625" customWidth="1"/>
+    <col min="14" max="14" width="53.36328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:20" x14ac:dyDescent="0.35">
@@ -4767,7 +4803,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>221</v>
       </c>
@@ -4784,10 +4820,13 @@
         <v>1</v>
       </c>
       <c r="F4" t="s">
-        <v>992</v>
+        <v>991</v>
       </c>
       <c r="G4">
         <v>1</v>
+      </c>
+      <c r="N4" t="s">
+        <v>995</v>
       </c>
       <c r="O4">
         <v>1</v>
@@ -4850,7 +4889,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>229</v>
       </c>
@@ -4867,10 +4906,13 @@
         <v>1</v>
       </c>
       <c r="F8" t="s">
-        <v>992</v>
+        <v>991</v>
       </c>
       <c r="G8">
         <v>1</v>
+      </c>
+      <c r="N8" t="s">
+        <v>988</v>
       </c>
       <c r="O8">
         <v>1</v>
@@ -4967,7 +5009,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>245</v>
       </c>
@@ -4984,16 +5026,19 @@
         <v>1</v>
       </c>
       <c r="F14" t="s">
-        <v>992</v>
+        <v>991</v>
       </c>
       <c r="G14">
-        <v>1</v>
+        <v>0</v>
+      </c>
+      <c r="N14" t="s">
+        <v>996</v>
       </c>
       <c r="O14">
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>248</v>
       </c>
@@ -5010,7 +5055,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>251</v>
       </c>
@@ -5027,7 +5072,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:18" hidden="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>254</v>
       </c>
@@ -5044,7 +5089,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:18" hidden="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>257</v>
       </c>
@@ -5149,7 +5194,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:18" hidden="1" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>274</v>
       </c>
@@ -5166,16 +5211,19 @@
         <v>1</v>
       </c>
       <c r="F24" t="s">
-        <v>992</v>
+        <v>991</v>
       </c>
       <c r="G24">
         <v>1</v>
       </c>
+      <c r="N24" t="s">
+        <v>1004</v>
+      </c>
       <c r="R24">
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:18" hidden="1" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>277</v>
       </c>
@@ -5192,16 +5240,19 @@
         <v>1</v>
       </c>
       <c r="F25" t="s">
-        <v>992</v>
+        <v>991</v>
       </c>
       <c r="G25">
-        <v>1</v>
+        <v>0</v>
+      </c>
+      <c r="N25" t="s">
+        <v>997</v>
       </c>
       <c r="R25">
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:18" hidden="1" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>280</v>
       </c>
@@ -5218,16 +5269,16 @@
         <v>1</v>
       </c>
       <c r="F26" t="s">
-        <v>992</v>
+        <v>991</v>
       </c>
       <c r="G26">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R26">
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:18" hidden="1" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>283</v>
       </c>
@@ -5244,16 +5295,16 @@
         <v>1</v>
       </c>
       <c r="F27" t="s">
-        <v>992</v>
+        <v>991</v>
       </c>
       <c r="G27">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R27">
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:18" hidden="1" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>286</v>
       </c>
@@ -5270,16 +5321,16 @@
         <v>1</v>
       </c>
       <c r="F28" t="s">
-        <v>992</v>
+        <v>991</v>
       </c>
       <c r="G28">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R28">
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:18" hidden="1" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>289</v>
       </c>
@@ -5296,10 +5347,10 @@
         <v>1</v>
       </c>
       <c r="F29" t="s">
-        <v>992</v>
+        <v>991</v>
       </c>
       <c r="G29">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R29">
         <v>1</v>
@@ -5345,10 +5396,10 @@
         <v>1</v>
       </c>
       <c r="F31" t="s">
-        <v>992</v>
+        <v>991</v>
       </c>
       <c r="G31">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P31">
         <v>1</v>
@@ -5803,7 +5854,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="57" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:18" hidden="1" x14ac:dyDescent="0.35">
       <c r="A57" t="s">
         <v>372</v>
       </c>
@@ -5820,10 +5871,10 @@
         <v>1</v>
       </c>
       <c r="F57" t="s">
-        <v>992</v>
+        <v>991</v>
       </c>
       <c r="G57">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R57">
         <v>1</v>
@@ -5846,7 +5897,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="59" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:18" hidden="1" x14ac:dyDescent="0.35">
       <c r="A59" t="s">
         <v>377</v>
       </c>
@@ -5863,10 +5914,10 @@
         <v>1</v>
       </c>
       <c r="F59" t="s">
-        <v>992</v>
+        <v>991</v>
       </c>
       <c r="G59">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R59">
         <v>1</v>
@@ -6025,7 +6076,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="69" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:18" hidden="1" x14ac:dyDescent="0.35">
       <c r="A69" t="s">
         <v>407</v>
       </c>
@@ -6045,7 +6096,7 @@
         <v>4</v>
       </c>
       <c r="G69">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R69">
         <v>1</v>
@@ -6085,7 +6136,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="72" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:18" hidden="1" x14ac:dyDescent="0.35">
       <c r="A72" t="s">
         <v>416</v>
       </c>
@@ -6102,7 +6153,7 @@
         <v>1</v>
       </c>
       <c r="F72" t="s">
-        <v>992</v>
+        <v>991</v>
       </c>
       <c r="G72">
         <v>1</v>
@@ -6128,7 +6179,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="74" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:18" hidden="1" x14ac:dyDescent="0.35">
       <c r="A74" t="s">
         <v>422</v>
       </c>
@@ -6145,10 +6196,13 @@
         <v>1</v>
       </c>
       <c r="F74" t="s">
-        <v>992</v>
+        <v>991</v>
       </c>
       <c r="G74">
         <v>1</v>
+      </c>
+      <c r="N74" t="s">
+        <v>998</v>
       </c>
       <c r="O74">
         <v>1</v>
@@ -6191,7 +6245,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="77" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:18" hidden="1" x14ac:dyDescent="0.35">
       <c r="A77" t="s">
         <v>430</v>
       </c>
@@ -6208,7 +6262,7 @@
         <v>1</v>
       </c>
       <c r="F77" t="s">
-        <v>992</v>
+        <v>991</v>
       </c>
       <c r="G77">
         <v>1</v>
@@ -6220,7 +6274,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="78" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:18" hidden="1" x14ac:dyDescent="0.35">
       <c r="A78" t="s">
         <v>433</v>
       </c>
@@ -6237,16 +6291,16 @@
         <v>1</v>
       </c>
       <c r="F78" t="s">
-        <v>992</v>
+        <v>991</v>
       </c>
       <c r="G78">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O78">
         <v>1</v>
       </c>
     </row>
-    <row r="79" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:18" hidden="1" x14ac:dyDescent="0.35">
       <c r="A79" t="s">
         <v>436</v>
       </c>
@@ -6263,16 +6317,16 @@
         <v>1</v>
       </c>
       <c r="F79" t="s">
-        <v>992</v>
+        <v>991</v>
       </c>
       <c r="G79">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O79">
         <v>1</v>
       </c>
     </row>
-    <row r="80" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:18" hidden="1" x14ac:dyDescent="0.35">
       <c r="A80" t="s">
         <v>439</v>
       </c>
@@ -6289,16 +6343,19 @@
         <v>1</v>
       </c>
       <c r="F80" t="s">
-        <v>992</v>
+        <v>991</v>
       </c>
       <c r="G80">
-        <v>1</v>
+        <v>0</v>
+      </c>
+      <c r="N80" t="s">
+        <v>999</v>
       </c>
       <c r="O80">
         <v>1</v>
       </c>
     </row>
-    <row r="81" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:19" hidden="1" x14ac:dyDescent="0.35">
       <c r="A81" t="s">
         <v>442</v>
       </c>
@@ -6315,7 +6372,7 @@
         <v>1</v>
       </c>
       <c r="F81" t="s">
-        <v>992</v>
+        <v>991</v>
       </c>
       <c r="G81">
         <v>1</v>
@@ -6326,7 +6383,7 @@
     </row>
     <row r="82" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A82" t="s">
-        <v>993</v>
+        <v>992</v>
       </c>
       <c r="B82" t="s">
         <v>445</v>
@@ -6341,10 +6398,10 @@
         <v>1</v>
       </c>
       <c r="F82" t="s">
-        <v>992</v>
+        <v>991</v>
       </c>
       <c r="G82">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P82">
         <v>1</v>
@@ -6367,16 +6424,16 @@
         <v>1</v>
       </c>
       <c r="F83" t="s">
-        <v>992</v>
+        <v>991</v>
       </c>
       <c r="G83">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P83">
         <v>1</v>
       </c>
     </row>
-    <row r="84" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:19" hidden="1" x14ac:dyDescent="0.35">
       <c r="A84" t="s">
         <v>450</v>
       </c>
@@ -6393,16 +6450,16 @@
         <v>1</v>
       </c>
       <c r="F84" t="s">
-        <v>992</v>
+        <v>991</v>
       </c>
       <c r="G84">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O84">
         <v>1</v>
       </c>
     </row>
-    <row r="85" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:19" hidden="1" x14ac:dyDescent="0.35">
       <c r="A85" t="s">
         <v>453</v>
       </c>
@@ -6419,16 +6476,19 @@
         <v>1</v>
       </c>
       <c r="F85" t="s">
-        <v>992</v>
+        <v>991</v>
       </c>
       <c r="G85">
-        <v>1</v>
+        <v>0</v>
+      </c>
+      <c r="N85" t="s">
+        <v>1000</v>
       </c>
       <c r="O85">
         <v>1</v>
       </c>
     </row>
-    <row r="86" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:19" hidden="1" x14ac:dyDescent="0.35">
       <c r="A86" t="s">
         <v>456</v>
       </c>
@@ -6445,10 +6505,13 @@
         <v>1</v>
       </c>
       <c r="F86" t="s">
-        <v>992</v>
+        <v>991</v>
       </c>
       <c r="G86">
-        <v>1</v>
+        <v>0</v>
+      </c>
+      <c r="N86" t="s">
+        <v>1000</v>
       </c>
       <c r="O86">
         <v>1</v>
@@ -6505,7 +6568,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="90" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:19" hidden="1" x14ac:dyDescent="0.35">
       <c r="A90" t="s">
         <v>468</v>
       </c>
@@ -6522,7 +6585,7 @@
         <v>1</v>
       </c>
       <c r="F90" t="s">
-        <v>992</v>
+        <v>991</v>
       </c>
       <c r="G90">
         <v>1</v>
@@ -6531,7 +6594,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="91" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:19" hidden="1" x14ac:dyDescent="0.35">
       <c r="A91" t="s">
         <v>471</v>
       </c>
@@ -6548,7 +6611,7 @@
         <v>1</v>
       </c>
       <c r="F91" t="s">
-        <v>992</v>
+        <v>991</v>
       </c>
       <c r="G91">
         <v>1</v>
@@ -6557,7 +6620,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="92" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:19" hidden="1" x14ac:dyDescent="0.35">
       <c r="A92" t="s">
         <v>474</v>
       </c>
@@ -6574,7 +6637,7 @@
         <v>1</v>
       </c>
       <c r="F92" t="s">
-        <v>992</v>
+        <v>991</v>
       </c>
       <c r="G92">
         <v>1</v>
@@ -6583,7 +6646,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="93" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:19" hidden="1" x14ac:dyDescent="0.35">
       <c r="A93" t="s">
         <v>477</v>
       </c>
@@ -6600,10 +6663,10 @@
         <v>1</v>
       </c>
       <c r="F93" t="s">
-        <v>992</v>
+        <v>991</v>
       </c>
       <c r="G93">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S93">
         <v>1</v>
@@ -6783,8 +6846,11 @@
       <c r="E101">
         <v>1</v>
       </c>
-      <c r="N101" t="s">
-        <v>988</v>
+      <c r="F101" t="s">
+        <v>991</v>
+      </c>
+      <c r="G101">
+        <v>1</v>
       </c>
       <c r="Q101">
         <v>1</v>
@@ -6826,8 +6892,11 @@
       <c r="E103">
         <v>1</v>
       </c>
-      <c r="N103" t="s">
-        <v>988</v>
+      <c r="F103" t="s">
+        <v>991</v>
+      </c>
+      <c r="G103">
+        <v>1</v>
       </c>
       <c r="Q103">
         <v>1</v>
@@ -7105,7 +7174,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="117" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="117" spans="1:19" hidden="1" x14ac:dyDescent="0.35">
       <c r="A117" t="s">
         <v>544</v>
       </c>
@@ -7122,10 +7191,10 @@
         <v>1</v>
       </c>
       <c r="F117" t="s">
-        <v>992</v>
+        <v>991</v>
       </c>
       <c r="G117">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q117">
         <v>1</v>
@@ -7313,11 +7382,17 @@
       <c r="E126">
         <v>1</v>
       </c>
+      <c r="F126" t="s">
+        <v>991</v>
+      </c>
+      <c r="G126">
+        <v>1</v>
+      </c>
       <c r="Q126">
         <v>1</v>
       </c>
     </row>
-    <row r="127" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="127" spans="1:19" hidden="1" x14ac:dyDescent="0.35">
       <c r="A127" t="s">
         <v>573</v>
       </c>
@@ -7334,7 +7409,7 @@
         <v>4</v>
       </c>
       <c r="G127">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q127">
         <v>1</v>
@@ -7443,7 +7518,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="133" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="133" spans="1:19" hidden="1" x14ac:dyDescent="0.35">
       <c r="A133" t="s">
         <v>589</v>
       </c>
@@ -7463,7 +7538,10 @@
         <v>4</v>
       </c>
       <c r="G133">
-        <v>1</v>
+        <v>0</v>
+      </c>
+      <c r="N133" t="s">
+        <v>1001</v>
       </c>
       <c r="Q133">
         <v>1</v>
@@ -7566,7 +7644,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="139" spans="1:19" hidden="1" x14ac:dyDescent="0.35">
+    <row r="139" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A139" t="s">
         <v>607</v>
       </c>
@@ -7586,7 +7664,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="140" spans="1:19" hidden="1" x14ac:dyDescent="0.35">
+    <row r="140" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A140" t="s">
         <v>610</v>
       </c>
@@ -7703,13 +7781,13 @@
         <v>1</v>
       </c>
       <c r="N145" t="s">
-        <v>990</v>
+        <v>989</v>
       </c>
       <c r="R145">
         <v>1</v>
       </c>
     </row>
-    <row r="146" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="146" spans="1:18" hidden="1" x14ac:dyDescent="0.35">
       <c r="A146" t="s">
         <v>628</v>
       </c>
@@ -7726,13 +7804,13 @@
         <v>1</v>
       </c>
       <c r="F146" t="s">
-        <v>992</v>
+        <v>991</v>
       </c>
       <c r="G146">
         <v>1</v>
       </c>
       <c r="N146" t="s">
-        <v>989</v>
+        <v>1002</v>
       </c>
       <c r="R146">
         <v>1</v>
@@ -8038,7 +8116,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="162" spans="1:18" hidden="1" x14ac:dyDescent="0.35">
+    <row r="162" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A162" t="s">
         <v>675</v>
       </c>
@@ -8344,7 +8422,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="177" spans="1:18" hidden="1" x14ac:dyDescent="0.35">
+    <row r="177" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A177" t="s">
         <v>717</v>
       </c>
@@ -8364,7 +8442,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="178" spans="1:18" hidden="1" x14ac:dyDescent="0.35">
+    <row r="178" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A178" t="s">
         <v>720</v>
       </c>
@@ -8380,11 +8458,17 @@
       <c r="E178">
         <v>1</v>
       </c>
+      <c r="F178" t="s">
+        <v>991</v>
+      </c>
+      <c r="G178">
+        <v>1</v>
+      </c>
       <c r="P178">
         <v>1</v>
       </c>
     </row>
-    <row r="179" spans="1:18" hidden="1" x14ac:dyDescent="0.35">
+    <row r="179" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A179" t="s">
         <v>723</v>
       </c>
@@ -8400,11 +8484,17 @@
       <c r="E179">
         <v>1</v>
       </c>
+      <c r="F179" t="s">
+        <v>991</v>
+      </c>
+      <c r="G179">
+        <v>1</v>
+      </c>
       <c r="P179">
         <v>1</v>
       </c>
     </row>
-    <row r="180" spans="1:18" hidden="1" x14ac:dyDescent="0.35">
+    <row r="180" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A180" t="s">
         <v>726</v>
       </c>
@@ -8418,7 +8508,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="181" spans="1:18" hidden="1" x14ac:dyDescent="0.35">
+    <row r="181" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A181" t="s">
         <v>728</v>
       </c>
@@ -8432,7 +8522,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="182" spans="1:18" hidden="1" x14ac:dyDescent="0.35">
+    <row r="182" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A182" t="s">
         <v>730</v>
       </c>
@@ -8452,7 +8542,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="183" spans="1:18" hidden="1" x14ac:dyDescent="0.35">
+    <row r="183" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A183" t="s">
         <v>733</v>
       </c>
@@ -8465,11 +8555,17 @@
       <c r="E183">
         <v>1</v>
       </c>
+      <c r="F183" t="s">
+        <v>991</v>
+      </c>
+      <c r="G183">
+        <v>1</v>
+      </c>
       <c r="P183">
         <v>1</v>
       </c>
     </row>
-    <row r="184" spans="1:18" hidden="1" x14ac:dyDescent="0.35">
+    <row r="184" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A184" t="s">
         <v>735</v>
       </c>
@@ -8483,7 +8579,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="185" spans="1:18" hidden="1" x14ac:dyDescent="0.35">
+    <row r="185" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A185" t="s">
         <v>737</v>
       </c>
@@ -8497,7 +8593,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="186" spans="1:18" hidden="1" x14ac:dyDescent="0.35">
+    <row r="186" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A186" t="s">
         <v>739</v>
       </c>
@@ -8511,7 +8607,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="187" spans="1:18" hidden="1" x14ac:dyDescent="0.35">
+    <row r="187" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A187" t="s">
         <v>741</v>
       </c>
@@ -8531,7 +8627,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="188" spans="1:18" hidden="1" x14ac:dyDescent="0.35">
+    <row r="188" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A188" t="s">
         <v>744</v>
       </c>
@@ -8551,7 +8647,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="189" spans="1:18" hidden="1" x14ac:dyDescent="0.35">
+    <row r="189" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A189" t="s">
         <v>747</v>
       </c>
@@ -8593,7 +8689,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="192" spans="1:18" hidden="1" x14ac:dyDescent="0.35">
+    <row r="192" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A192" t="s">
         <v>752</v>
       </c>
@@ -8701,7 +8797,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="198" spans="1:19" hidden="1" x14ac:dyDescent="0.35">
+    <row r="198" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A198" t="s">
         <v>768</v>
       </c>
@@ -8721,7 +8817,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="199" spans="1:19" hidden="1" x14ac:dyDescent="0.35">
+    <row r="199" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A199" t="s">
         <v>771</v>
       </c>
@@ -8737,11 +8833,17 @@
       <c r="E199">
         <v>1</v>
       </c>
+      <c r="F199" t="s">
+        <v>991</v>
+      </c>
+      <c r="G199">
+        <v>1</v>
+      </c>
       <c r="P199">
         <v>1</v>
       </c>
     </row>
-    <row r="200" spans="1:19" hidden="1" x14ac:dyDescent="0.35">
+    <row r="200" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A200" t="s">
         <v>774</v>
       </c>
@@ -8757,11 +8859,17 @@
       <c r="E200">
         <v>1</v>
       </c>
+      <c r="F200" t="s">
+        <v>991</v>
+      </c>
+      <c r="G200">
+        <v>1</v>
+      </c>
       <c r="P200">
         <v>1</v>
       </c>
     </row>
-    <row r="201" spans="1:19" hidden="1" x14ac:dyDescent="0.35">
+    <row r="201" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A201" t="s">
         <v>777</v>
       </c>
@@ -8818,7 +8926,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="204" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="204" spans="1:19" hidden="1" x14ac:dyDescent="0.35">
       <c r="A204" t="s">
         <v>786</v>
       </c>
@@ -8832,7 +8940,7 @@
         <v>1</v>
       </c>
       <c r="F204" t="s">
-        <v>992</v>
+        <v>991</v>
       </c>
       <c r="G204">
         <v>1</v>
@@ -8875,7 +8983,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="207" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="207" spans="1:19" hidden="1" x14ac:dyDescent="0.35">
       <c r="A207" t="s">
         <v>793</v>
       </c>
@@ -8889,10 +8997,10 @@
         <v>1</v>
       </c>
       <c r="F207" t="s">
-        <v>992</v>
+        <v>991</v>
       </c>
       <c r="G207">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R207">
         <v>1</v>
@@ -8915,7 +9023,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="209" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="209" spans="1:18" hidden="1" x14ac:dyDescent="0.35">
       <c r="A209" t="s">
         <v>798</v>
       </c>
@@ -8929,10 +9037,13 @@
         <v>1</v>
       </c>
       <c r="F209" t="s">
-        <v>992</v>
+        <v>991</v>
       </c>
       <c r="G209">
         <v>1</v>
+      </c>
+      <c r="N209" t="s">
+        <v>1005</v>
       </c>
       <c r="R209">
         <v>1</v>
@@ -8952,7 +9063,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="211" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="211" spans="1:18" hidden="1" x14ac:dyDescent="0.35">
       <c r="A211" t="s">
         <v>802</v>
       </c>
@@ -8966,16 +9077,16 @@
         <v>1</v>
       </c>
       <c r="F211" t="s">
-        <v>992</v>
+        <v>991</v>
       </c>
       <c r="G211">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R211">
         <v>1</v>
       </c>
     </row>
-    <row r="212" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="212" spans="1:18" hidden="1" x14ac:dyDescent="0.35">
       <c r="A212" t="s">
         <v>804</v>
       </c>
@@ -8989,10 +9100,10 @@
         <v>1</v>
       </c>
       <c r="F212" t="s">
-        <v>992</v>
+        <v>991</v>
       </c>
       <c r="G212">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R212">
         <v>1</v>
@@ -9012,7 +9123,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="214" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="214" spans="1:18" hidden="1" x14ac:dyDescent="0.35">
       <c r="A214" t="s">
         <v>808</v>
       </c>
@@ -9026,16 +9137,16 @@
         <v>1</v>
       </c>
       <c r="F214" t="s">
-        <v>992</v>
+        <v>991</v>
       </c>
       <c r="G214">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R214">
         <v>1</v>
       </c>
     </row>
-    <row r="215" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="215" spans="1:18" hidden="1" x14ac:dyDescent="0.35">
       <c r="A215" t="s">
         <v>810</v>
       </c>
@@ -9049,10 +9160,13 @@
         <v>1</v>
       </c>
       <c r="F215" t="s">
-        <v>992</v>
+        <v>991</v>
       </c>
       <c r="G215">
         <v>1</v>
+      </c>
+      <c r="N215" t="s">
+        <v>1005</v>
       </c>
       <c r="R215">
         <v>1</v>
@@ -9075,7 +9189,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="217" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="217" spans="1:18" hidden="1" x14ac:dyDescent="0.35">
       <c r="A217" t="s">
         <v>815</v>
       </c>
@@ -9092,7 +9206,7 @@
         <v>1</v>
       </c>
       <c r="F217" t="s">
-        <v>992</v>
+        <v>991</v>
       </c>
       <c r="G217">
         <v>1</v>
@@ -9118,7 +9232,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="219" spans="1:18" hidden="1" x14ac:dyDescent="0.35">
+    <row r="219" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A219" t="s">
         <v>821</v>
       </c>
@@ -9155,7 +9269,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="221" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="221" spans="1:18" hidden="1" x14ac:dyDescent="0.35">
       <c r="A221" t="s">
         <v>826</v>
       </c>
@@ -9172,10 +9286,10 @@
         <v>1</v>
       </c>
       <c r="F221" t="s">
-        <v>992</v>
+        <v>991</v>
       </c>
       <c r="G221">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R221">
         <v>1</v>
@@ -9201,7 +9315,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="223" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="223" spans="1:18" hidden="1" x14ac:dyDescent="0.35">
       <c r="A223" t="s">
         <v>832</v>
       </c>
@@ -9218,7 +9332,7 @@
         <v>1</v>
       </c>
       <c r="F223" t="s">
-        <v>992</v>
+        <v>991</v>
       </c>
       <c r="G223">
         <v>1</v>
@@ -9227,7 +9341,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="224" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="224" spans="1:18" hidden="1" x14ac:dyDescent="0.35">
       <c r="A224" t="s">
         <v>835</v>
       </c>
@@ -9244,10 +9358,10 @@
         <v>1</v>
       </c>
       <c r="F224" t="s">
-        <v>992</v>
+        <v>991</v>
       </c>
       <c r="G224">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R224">
         <v>1</v>
@@ -9270,7 +9384,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="226" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="226" spans="1:18" hidden="1" x14ac:dyDescent="0.35">
       <c r="A226" t="s">
         <v>840</v>
       </c>
@@ -9287,16 +9401,16 @@
         <v>1</v>
       </c>
       <c r="F226" t="s">
-        <v>992</v>
+        <v>991</v>
       </c>
       <c r="G226">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R226">
         <v>1</v>
       </c>
     </row>
-    <row r="227" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="227" spans="1:18" hidden="1" x14ac:dyDescent="0.35">
       <c r="A227" t="s">
         <v>843</v>
       </c>
@@ -9310,7 +9424,7 @@
         <v>1</v>
       </c>
       <c r="F227" t="s">
-        <v>992</v>
+        <v>991</v>
       </c>
       <c r="G227">
         <v>1</v>
@@ -9333,7 +9447,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="229" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="229" spans="1:18" hidden="1" x14ac:dyDescent="0.35">
       <c r="A229" t="s">
         <v>847</v>
       </c>
@@ -9350,7 +9464,7 @@
         <v>4</v>
       </c>
       <c r="G229">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R229">
         <v>1</v>
@@ -9373,7 +9487,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="231" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="231" spans="1:18" hidden="1" x14ac:dyDescent="0.35">
       <c r="A231" t="s">
         <v>851</v>
       </c>
@@ -9387,7 +9501,7 @@
         <v>1</v>
       </c>
       <c r="F231" t="s">
-        <v>992</v>
+        <v>991</v>
       </c>
       <c r="G231">
         <v>1</v>
@@ -9396,7 +9510,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="232" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="232" spans="1:18" hidden="1" x14ac:dyDescent="0.35">
       <c r="A232" t="s">
         <v>853</v>
       </c>
@@ -9413,10 +9527,10 @@
         <v>1</v>
       </c>
       <c r="F232" t="s">
-        <v>992</v>
+        <v>991</v>
       </c>
       <c r="G232">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R232">
         <v>1</v>
@@ -9459,7 +9573,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="235" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="235" spans="1:18" hidden="1" x14ac:dyDescent="0.35">
       <c r="A235" t="s">
         <v>861</v>
       </c>
@@ -9476,10 +9590,10 @@
         <v>1</v>
       </c>
       <c r="F235" t="s">
-        <v>992</v>
+        <v>991</v>
       </c>
       <c r="G235">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R235">
         <v>1</v>
@@ -9522,7 +9636,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="238" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="238" spans="1:18" hidden="1" x14ac:dyDescent="0.35">
       <c r="A238" t="s">
         <v>869</v>
       </c>
@@ -9536,7 +9650,7 @@
         <v>1</v>
       </c>
       <c r="F238" t="s">
-        <v>992</v>
+        <v>991</v>
       </c>
       <c r="G238">
         <v>1</v>
@@ -9545,7 +9659,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="239" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="239" spans="1:18" hidden="1" x14ac:dyDescent="0.35">
       <c r="A239" t="s">
         <v>871</v>
       </c>
@@ -9559,19 +9673,19 @@
         <v>1</v>
       </c>
       <c r="F239" t="s">
-        <v>992</v>
+        <v>991</v>
       </c>
       <c r="G239">
         <v>1</v>
       </c>
       <c r="N239" t="s">
-        <v>991</v>
+        <v>990</v>
       </c>
       <c r="R239">
         <v>1</v>
       </c>
     </row>
-    <row r="240" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="240" spans="1:18" hidden="1" x14ac:dyDescent="0.35">
       <c r="A240" t="s">
         <v>873</v>
       </c>
@@ -9588,10 +9702,10 @@
         <v>1</v>
       </c>
       <c r="F240" t="s">
-        <v>992</v>
+        <v>991</v>
       </c>
       <c r="G240">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R240">
         <v>1</v>
@@ -9631,7 +9745,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="243" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="243" spans="1:19" hidden="1" x14ac:dyDescent="0.35">
       <c r="A243" t="s">
         <v>882</v>
       </c>
@@ -9648,13 +9762,13 @@
         <v>4</v>
       </c>
       <c r="G243">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S243">
         <v>1</v>
       </c>
     </row>
-    <row r="244" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="244" spans="1:19" hidden="1" x14ac:dyDescent="0.35">
       <c r="A244" t="s">
         <v>884</v>
       </c>
@@ -9668,16 +9782,16 @@
         <v>1</v>
       </c>
       <c r="F244" t="s">
-        <v>992</v>
+        <v>991</v>
       </c>
       <c r="G244">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R244">
         <v>1</v>
       </c>
     </row>
-    <row r="245" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="245" spans="1:19" hidden="1" x14ac:dyDescent="0.35">
       <c r="A245" t="s">
         <v>886</v>
       </c>
@@ -9691,7 +9805,7 @@
         <v>1</v>
       </c>
       <c r="F245" t="s">
-        <v>992</v>
+        <v>991</v>
       </c>
       <c r="G245">
         <v>1</v>
@@ -9700,7 +9814,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="246" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="246" spans="1:19" hidden="1" x14ac:dyDescent="0.35">
       <c r="A246" t="s">
         <v>887</v>
       </c>
@@ -9714,7 +9828,7 @@
         <v>1</v>
       </c>
       <c r="F246" t="s">
-        <v>992</v>
+        <v>991</v>
       </c>
       <c r="G246">
         <v>1</v>
@@ -9723,7 +9837,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="247" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="247" spans="1:19" hidden="1" x14ac:dyDescent="0.35">
       <c r="A247" t="s">
         <v>889</v>
       </c>
@@ -9740,7 +9854,7 @@
         <v>1</v>
       </c>
       <c r="F247" t="s">
-        <v>992</v>
+        <v>991</v>
       </c>
       <c r="G247">
         <v>1</v>
@@ -9749,7 +9863,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="248" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="248" spans="1:19" hidden="1" x14ac:dyDescent="0.35">
       <c r="A248" t="s">
         <v>892</v>
       </c>
@@ -9766,7 +9880,7 @@
         <v>1</v>
       </c>
       <c r="F248" t="s">
-        <v>992</v>
+        <v>991</v>
       </c>
       <c r="G248">
         <v>1</v>
@@ -9775,7 +9889,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="249" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="249" spans="1:19" hidden="1" x14ac:dyDescent="0.35">
       <c r="A249" t="s">
         <v>895</v>
       </c>
@@ -9792,7 +9906,7 @@
         <v>1</v>
       </c>
       <c r="F249" t="s">
-        <v>992</v>
+        <v>991</v>
       </c>
       <c r="G249">
         <v>1</v>
@@ -9801,7 +9915,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="250" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="250" spans="1:19" hidden="1" x14ac:dyDescent="0.35">
       <c r="A250" t="s">
         <v>898</v>
       </c>
@@ -9815,16 +9929,16 @@
         <v>1</v>
       </c>
       <c r="F250" t="s">
-        <v>992</v>
+        <v>991</v>
       </c>
       <c r="G250">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O250">
         <v>1</v>
       </c>
     </row>
-    <row r="251" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="251" spans="1:19" hidden="1" x14ac:dyDescent="0.35">
       <c r="A251" t="s">
         <v>900</v>
       </c>
@@ -9838,13 +9952,16 @@
         <v>1</v>
       </c>
       <c r="F251" t="s">
-        <v>992</v>
+        <v>991</v>
       </c>
       <c r="G251">
         <v>1</v>
       </c>
-    </row>
-    <row r="252" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="S251">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="252" spans="1:19" hidden="1" x14ac:dyDescent="0.35">
       <c r="A252" t="s">
         <v>902</v>
       </c>
@@ -9861,16 +9978,16 @@
         <v>1</v>
       </c>
       <c r="F252" t="s">
-        <v>992</v>
+        <v>991</v>
       </c>
       <c r="G252">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O252">
         <v>1</v>
       </c>
     </row>
-    <row r="253" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="253" spans="1:19" hidden="1" x14ac:dyDescent="0.35">
       <c r="A253" t="s">
         <v>905</v>
       </c>
@@ -9884,10 +10001,13 @@
         <v>1</v>
       </c>
       <c r="F253" t="s">
-        <v>992</v>
+        <v>991</v>
       </c>
       <c r="G253">
         <v>1</v>
+      </c>
+      <c r="N253" t="s">
+        <v>1003</v>
       </c>
       <c r="O253">
         <v>1</v>
@@ -9907,7 +10027,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="255" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="255" spans="1:19" hidden="1" x14ac:dyDescent="0.35">
       <c r="A255" t="s">
         <v>909</v>
       </c>
@@ -9924,10 +10044,13 @@
         <v>1</v>
       </c>
       <c r="F255" t="s">
-        <v>992</v>
+        <v>991</v>
       </c>
       <c r="G255">
         <v>1</v>
+      </c>
+      <c r="N255" t="s">
+        <v>1006</v>
       </c>
       <c r="Q255">
         <v>1</v>
@@ -9964,7 +10087,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="258" spans="1:19" hidden="1" x14ac:dyDescent="0.35">
+    <row r="258" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A258" t="s">
         <v>916</v>
       </c>
@@ -10001,7 +10124,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="260" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="260" spans="1:19" hidden="1" x14ac:dyDescent="0.35">
       <c r="A260" t="s">
         <v>921</v>
       </c>
@@ -10015,7 +10138,7 @@
         <v>1</v>
       </c>
       <c r="F260" t="s">
-        <v>992</v>
+        <v>991</v>
       </c>
       <c r="G260">
         <v>1</v>
@@ -10024,12 +10147,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="261" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="261" spans="1:19" hidden="1" x14ac:dyDescent="0.35">
       <c r="A261" t="s">
+        <v>993</v>
+      </c>
+      <c r="B261" t="s">
         <v>994</v>
-      </c>
-      <c r="B261" t="s">
-        <v>995</v>
       </c>
       <c r="D261">
         <v>1</v>
@@ -10041,13 +10164,13 @@
         <v>4</v>
       </c>
       <c r="G261">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q261">
         <v>1</v>
       </c>
     </row>
-    <row r="262" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="262" spans="1:19" hidden="1" x14ac:dyDescent="0.35">
       <c r="A262" t="s">
         <v>923</v>
       </c>
@@ -10096,7 +10219,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="264" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="264" spans="1:19" hidden="1" x14ac:dyDescent="0.35">
       <c r="A264" t="s">
         <v>929</v>
       </c>
@@ -10113,7 +10236,7 @@
         <v>1</v>
       </c>
       <c r="F264" t="s">
-        <v>992</v>
+        <v>991</v>
       </c>
       <c r="G264">
         <v>1</v>
@@ -10145,7 +10268,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="266" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="266" spans="1:19" hidden="1" x14ac:dyDescent="0.35">
       <c r="A266" t="s">
         <v>935</v>
       </c>
@@ -10162,16 +10285,16 @@
         <v>1</v>
       </c>
       <c r="F266" t="s">
-        <v>992</v>
+        <v>991</v>
       </c>
       <c r="G266">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R266">
         <v>1</v>
       </c>
     </row>
-    <row r="267" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="267" spans="1:19" hidden="1" x14ac:dyDescent="0.35">
       <c r="A267" t="s">
         <v>938</v>
       </c>
@@ -10185,10 +10308,13 @@
         <v>1</v>
       </c>
       <c r="F267" t="s">
-        <v>992</v>
+        <v>991</v>
       </c>
       <c r="G267">
         <v>1</v>
+      </c>
+      <c r="N267" t="s">
+        <v>1007</v>
       </c>
       <c r="R267">
         <v>1</v>
@@ -10214,7 +10340,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="269" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="269" spans="1:19" hidden="1" x14ac:dyDescent="0.35">
       <c r="A269" t="s">
         <v>942</v>
       </c>
@@ -10231,16 +10357,16 @@
         <v>1</v>
       </c>
       <c r="F269" t="s">
-        <v>992</v>
+        <v>991</v>
       </c>
       <c r="G269">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R269">
         <v>1</v>
       </c>
     </row>
-    <row r="270" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="270" spans="1:19" hidden="1" x14ac:dyDescent="0.35">
       <c r="A270" t="s">
         <v>944</v>
       </c>
@@ -10260,7 +10386,7 @@
         <v>4</v>
       </c>
       <c r="G270">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R270">
         <v>1</v>
@@ -10289,7 +10415,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="272" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="272" spans="1:19" hidden="1" x14ac:dyDescent="0.35">
       <c r="A272" t="s">
         <v>948</v>
       </c>
@@ -10306,7 +10432,7 @@
         <v>1</v>
       </c>
       <c r="F272" t="s">
-        <v>992</v>
+        <v>991</v>
       </c>
       <c r="G272">
         <v>1</v>
@@ -10315,7 +10441,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="273" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="273" spans="1:19" hidden="1" x14ac:dyDescent="0.35">
       <c r="A273" t="s">
         <v>950</v>
       </c>
@@ -10332,7 +10458,7 @@
         <v>1</v>
       </c>
       <c r="F273" t="s">
-        <v>992</v>
+        <v>991</v>
       </c>
       <c r="G273">
         <v>1</v>
@@ -10341,7 +10467,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="274" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="274" spans="1:19" hidden="1" x14ac:dyDescent="0.35">
       <c r="A274" t="s">
         <v>952</v>
       </c>
@@ -10358,16 +10484,16 @@
         <v>1</v>
       </c>
       <c r="F274" t="s">
-        <v>992</v>
+        <v>991</v>
       </c>
       <c r="G274">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S274">
         <v>1</v>
       </c>
     </row>
-    <row r="275" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="275" spans="1:19" hidden="1" x14ac:dyDescent="0.35">
       <c r="A275" t="s">
         <v>955</v>
       </c>
@@ -10384,10 +10510,10 @@
         <v>1</v>
       </c>
       <c r="F275" t="s">
-        <v>992</v>
+        <v>991</v>
       </c>
       <c r="G275">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S275">
         <v>1</v>
@@ -10407,7 +10533,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="277" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="277" spans="1:19" hidden="1" x14ac:dyDescent="0.35">
       <c r="A277" t="s">
         <v>960</v>
       </c>
@@ -10424,10 +10550,10 @@
         <v>1</v>
       </c>
       <c r="F277" t="s">
-        <v>992</v>
+        <v>991</v>
       </c>
       <c r="G277">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R277">
         <v>1</v>
@@ -10493,7 +10619,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="281" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="281" spans="1:19" hidden="1" x14ac:dyDescent="0.35">
       <c r="A281" t="s">
         <v>971</v>
       </c>
@@ -10510,7 +10636,7 @@
         <v>1</v>
       </c>
       <c r="F281" t="s">
-        <v>992</v>
+        <v>991</v>
       </c>
       <c r="G281">
         <v>1</v>
@@ -10536,7 +10662,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="283" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="283" spans="1:19" hidden="1" x14ac:dyDescent="0.35">
       <c r="A283" t="s">
         <v>977</v>
       </c>
@@ -10556,13 +10682,13 @@
         <v>4</v>
       </c>
       <c r="G283">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O283">
         <v>1</v>
       </c>
     </row>
-    <row r="284" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="284" spans="1:19" hidden="1" x14ac:dyDescent="0.35">
       <c r="A284" t="s">
         <v>982</v>
       </c>
@@ -10579,20 +10705,18 @@
         <v>1</v>
       </c>
       <c r="F284" t="s">
-        <v>992</v>
+        <v>991</v>
       </c>
       <c r="G284">
+        <v>1</v>
+      </c>
+      <c r="S284">
         <v>1</v>
       </c>
     </row>
   </sheetData>
   <autoFilter ref="A1:T284" xr:uid="{00000000-0001-0000-0200-000000000000}">
-    <filterColumn colId="4">
-      <customFilters>
-        <customFilter operator="notEqual" val=" "/>
-      </customFilters>
-    </filterColumn>
-    <filterColumn colId="5">
+    <filterColumn colId="15">
       <customFilters>
         <customFilter operator="notEqual" val=" "/>
       </customFilters>

</xml_diff>

<commit_message>
added recodings for pca script
</commit_message>
<xml_diff>
--- a/pathways workbook - ethiopia 2016.xlsx
+++ b/pathways workbook - ethiopia 2016.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://bmgf-my.sharepoint.com/personal/jeremy_cooper_gatesfoundation_org/Documents/scenario_dhs_ethiopia_2016/workshop_prep/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://bmgf-my.sharepoint.com/personal/jeremy_cooper_gatesfoundation_org/Documents/Documents/GitHub/pathways-segmentation-public/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="683" documentId="11_A09B48BC4F10D9CFB369C71317FDCB2BF82E9003" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{ECCB6027-FA62-4571-B6AA-FDD258EB60E6}"/>
+  <xr:revisionPtr revIDLastSave="1005" documentId="11_A09B48BC4F10D9CFB369C71317FDCB2BF82E9003" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{172D8825-26AE-4EE9-90B1-A3BC13DD604C}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11620" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1191" uniqueCount="996">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1212" uniqueCount="1008">
   <si>
     <t>domains</t>
   </si>
@@ -3008,9 +3008,6 @@
     <t>check</t>
   </si>
   <si>
-    <t>recode</t>
-  </si>
-  <si>
     <t xml:space="preserve">this drops because jd.index.cat is fixed </t>
   </si>
   <si>
@@ -3027,6 +3024,45 @@
   </si>
   <si>
     <t>HH Wboth</t>
+  </si>
+  <si>
+    <t>&lt;18, 18-25, 25+</t>
+  </si>
+  <si>
+    <t>using ed.level</t>
+  </si>
+  <si>
+    <t>collapse not partnered/other</t>
+  </si>
+  <si>
+    <t>combine secondary + higher</t>
+  </si>
+  <si>
+    <t>using polygamy</t>
+  </si>
+  <si>
+    <t>using Y/N variable</t>
+  </si>
+  <si>
+    <t>add HH Sanitation</t>
+  </si>
+  <si>
+    <t>recode (looks good)</t>
+  </si>
+  <si>
+    <t>fix</t>
+  </si>
+  <si>
+    <t>collapse not partnered/other, respondent and huband/partner</t>
+  </si>
+  <si>
+    <t>collapse 0 into 0-1</t>
+  </si>
+  <si>
+    <t>categorical (0, 1-2, 3-4)</t>
+  </si>
+  <si>
+    <t>0, 1-3, 4+</t>
   </si>
 </sst>
 </file>
@@ -3436,7 +3472,7 @@
   <dimension ref="A1:H72"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C42" sqref="C42"/>
+      <selection activeCell="A3" sqref="A3:A72"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4644,7 +4680,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F24" sqref="A1:T284"/>
+      <selection pane="bottomLeft" activeCell="A267" sqref="A267"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="74" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4662,7 +4698,7 @@
     <col min="11" max="11" width="15.6328125" hidden="1" customWidth="1"/>
     <col min="12" max="12" width="18.36328125" hidden="1" customWidth="1"/>
     <col min="13" max="13" width="19.6328125" hidden="1" customWidth="1"/>
-    <col min="14" max="14" width="13.90625" customWidth="1"/>
+    <col min="14" max="14" width="53.36328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:20" x14ac:dyDescent="0.35">
@@ -4784,10 +4820,13 @@
         <v>1</v>
       </c>
       <c r="F4" t="s">
-        <v>992</v>
+        <v>991</v>
       </c>
       <c r="G4">
         <v>1</v>
+      </c>
+      <c r="N4" t="s">
+        <v>995</v>
       </c>
       <c r="O4">
         <v>1</v>
@@ -4867,10 +4906,13 @@
         <v>1</v>
       </c>
       <c r="F8" t="s">
-        <v>992</v>
+        <v>991</v>
       </c>
       <c r="G8">
         <v>1</v>
+      </c>
+      <c r="N8" t="s">
+        <v>988</v>
       </c>
       <c r="O8">
         <v>1</v>
@@ -4967,7 +5009,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>245</v>
       </c>
@@ -4984,10 +5026,13 @@
         <v>1</v>
       </c>
       <c r="F14" t="s">
-        <v>992</v>
+        <v>991</v>
       </c>
       <c r="G14">
-        <v>1</v>
+        <v>0</v>
+      </c>
+      <c r="N14" t="s">
+        <v>996</v>
       </c>
       <c r="O14">
         <v>1</v>
@@ -5166,16 +5211,19 @@
         <v>1</v>
       </c>
       <c r="F24" t="s">
-        <v>992</v>
+        <v>991</v>
       </c>
       <c r="G24">
         <v>1</v>
       </c>
+      <c r="N24" t="s">
+        <v>1004</v>
+      </c>
       <c r="R24">
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:18" hidden="1" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>277</v>
       </c>
@@ -5192,16 +5240,19 @@
         <v>1</v>
       </c>
       <c r="F25" t="s">
-        <v>992</v>
+        <v>991</v>
       </c>
       <c r="G25">
-        <v>1</v>
+        <v>0</v>
+      </c>
+      <c r="N25" t="s">
+        <v>997</v>
       </c>
       <c r="R25">
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:18" hidden="1" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>280</v>
       </c>
@@ -5218,16 +5269,16 @@
         <v>1</v>
       </c>
       <c r="F26" t="s">
-        <v>992</v>
+        <v>991</v>
       </c>
       <c r="G26">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R26">
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:18" hidden="1" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>283</v>
       </c>
@@ -5244,16 +5295,16 @@
         <v>1</v>
       </c>
       <c r="F27" t="s">
-        <v>992</v>
+        <v>991</v>
       </c>
       <c r="G27">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R27">
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:18" hidden="1" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>286</v>
       </c>
@@ -5270,16 +5321,16 @@
         <v>1</v>
       </c>
       <c r="F28" t="s">
-        <v>992</v>
+        <v>991</v>
       </c>
       <c r="G28">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R28">
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:18" hidden="1" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>289</v>
       </c>
@@ -5296,10 +5347,10 @@
         <v>1</v>
       </c>
       <c r="F29" t="s">
-        <v>992</v>
+        <v>991</v>
       </c>
       <c r="G29">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R29">
         <v>1</v>
@@ -5328,7 +5379,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:18" hidden="1" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
         <v>295</v>
       </c>
@@ -5345,10 +5396,10 @@
         <v>1</v>
       </c>
       <c r="F31" t="s">
-        <v>992</v>
+        <v>991</v>
       </c>
       <c r="G31">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P31">
         <v>1</v>
@@ -5803,7 +5854,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="57" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:18" hidden="1" x14ac:dyDescent="0.35">
       <c r="A57" t="s">
         <v>372</v>
       </c>
@@ -5820,10 +5871,10 @@
         <v>1</v>
       </c>
       <c r="F57" t="s">
-        <v>992</v>
+        <v>991</v>
       </c>
       <c r="G57">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R57">
         <v>1</v>
@@ -5846,7 +5897,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="59" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:18" hidden="1" x14ac:dyDescent="0.35">
       <c r="A59" t="s">
         <v>377</v>
       </c>
@@ -5863,10 +5914,10 @@
         <v>1</v>
       </c>
       <c r="F59" t="s">
-        <v>992</v>
+        <v>991</v>
       </c>
       <c r="G59">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R59">
         <v>1</v>
@@ -6025,7 +6076,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="69" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:18" hidden="1" x14ac:dyDescent="0.35">
       <c r="A69" t="s">
         <v>407</v>
       </c>
@@ -6045,7 +6096,7 @@
         <v>4</v>
       </c>
       <c r="G69">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R69">
         <v>1</v>
@@ -6085,7 +6136,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="72" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:18" hidden="1" x14ac:dyDescent="0.35">
       <c r="A72" t="s">
         <v>416</v>
       </c>
@@ -6102,7 +6153,7 @@
         <v>1</v>
       </c>
       <c r="F72" t="s">
-        <v>992</v>
+        <v>991</v>
       </c>
       <c r="G72">
         <v>1</v>
@@ -6145,10 +6196,13 @@
         <v>1</v>
       </c>
       <c r="F74" t="s">
-        <v>992</v>
+        <v>991</v>
       </c>
       <c r="G74">
         <v>1</v>
+      </c>
+      <c r="N74" t="s">
+        <v>998</v>
       </c>
       <c r="O74">
         <v>1</v>
@@ -6208,7 +6262,7 @@
         <v>1</v>
       </c>
       <c r="F77" t="s">
-        <v>992</v>
+        <v>991</v>
       </c>
       <c r="G77">
         <v>1</v>
@@ -6220,7 +6274,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="78" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:18" hidden="1" x14ac:dyDescent="0.35">
       <c r="A78" t="s">
         <v>433</v>
       </c>
@@ -6237,16 +6291,16 @@
         <v>1</v>
       </c>
       <c r="F78" t="s">
-        <v>992</v>
+        <v>991</v>
       </c>
       <c r="G78">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O78">
         <v>1</v>
       </c>
     </row>
-    <row r="79" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:18" hidden="1" x14ac:dyDescent="0.35">
       <c r="A79" t="s">
         <v>436</v>
       </c>
@@ -6263,16 +6317,16 @@
         <v>1</v>
       </c>
       <c r="F79" t="s">
-        <v>992</v>
+        <v>991</v>
       </c>
       <c r="G79">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O79">
         <v>1</v>
       </c>
     </row>
-    <row r="80" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:18" hidden="1" x14ac:dyDescent="0.35">
       <c r="A80" t="s">
         <v>439</v>
       </c>
@@ -6289,16 +6343,19 @@
         <v>1</v>
       </c>
       <c r="F80" t="s">
-        <v>992</v>
+        <v>991</v>
       </c>
       <c r="G80">
-        <v>1</v>
+        <v>0</v>
+      </c>
+      <c r="N80" t="s">
+        <v>999</v>
       </c>
       <c r="O80">
         <v>1</v>
       </c>
     </row>
-    <row r="81" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:19" hidden="1" x14ac:dyDescent="0.35">
       <c r="A81" t="s">
         <v>442</v>
       </c>
@@ -6315,18 +6372,18 @@
         <v>1</v>
       </c>
       <c r="F81" t="s">
+        <v>991</v>
+      </c>
+      <c r="G81">
+        <v>1</v>
+      </c>
+      <c r="Q81">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="82" spans="1:19" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A82" t="s">
         <v>992</v>
-      </c>
-      <c r="G81">
-        <v>1</v>
-      </c>
-      <c r="Q81">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="82" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A82" t="s">
-        <v>993</v>
       </c>
       <c r="B82" t="s">
         <v>445</v>
@@ -6341,16 +6398,16 @@
         <v>1</v>
       </c>
       <c r="F82" t="s">
-        <v>992</v>
+        <v>991</v>
       </c>
       <c r="G82">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P82">
         <v>1</v>
       </c>
     </row>
-    <row r="83" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:19" hidden="1" x14ac:dyDescent="0.35">
       <c r="A83" t="s">
         <v>447</v>
       </c>
@@ -6367,16 +6424,16 @@
         <v>1</v>
       </c>
       <c r="F83" t="s">
-        <v>992</v>
+        <v>991</v>
       </c>
       <c r="G83">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P83">
         <v>1</v>
       </c>
     </row>
-    <row r="84" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:19" hidden="1" x14ac:dyDescent="0.35">
       <c r="A84" t="s">
         <v>450</v>
       </c>
@@ -6393,16 +6450,16 @@
         <v>1</v>
       </c>
       <c r="F84" t="s">
-        <v>992</v>
+        <v>991</v>
       </c>
       <c r="G84">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O84">
         <v>1</v>
       </c>
     </row>
-    <row r="85" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:19" hidden="1" x14ac:dyDescent="0.35">
       <c r="A85" t="s">
         <v>453</v>
       </c>
@@ -6419,16 +6476,19 @@
         <v>1</v>
       </c>
       <c r="F85" t="s">
-        <v>992</v>
+        <v>991</v>
       </c>
       <c r="G85">
-        <v>1</v>
+        <v>0</v>
+      </c>
+      <c r="N85" t="s">
+        <v>1000</v>
       </c>
       <c r="O85">
         <v>1</v>
       </c>
     </row>
-    <row r="86" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:19" hidden="1" x14ac:dyDescent="0.35">
       <c r="A86" t="s">
         <v>456</v>
       </c>
@@ -6445,10 +6505,13 @@
         <v>1</v>
       </c>
       <c r="F86" t="s">
-        <v>992</v>
+        <v>991</v>
       </c>
       <c r="G86">
-        <v>1</v>
+        <v>0</v>
+      </c>
+      <c r="N86" t="s">
+        <v>1000</v>
       </c>
       <c r="O86">
         <v>1</v>
@@ -6505,7 +6568,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="90" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:19" hidden="1" x14ac:dyDescent="0.35">
       <c r="A90" t="s">
         <v>468</v>
       </c>
@@ -6522,7 +6585,7 @@
         <v>1</v>
       </c>
       <c r="F90" t="s">
-        <v>992</v>
+        <v>991</v>
       </c>
       <c r="G90">
         <v>1</v>
@@ -6531,7 +6594,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="91" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:19" hidden="1" x14ac:dyDescent="0.35">
       <c r="A91" t="s">
         <v>471</v>
       </c>
@@ -6548,7 +6611,7 @@
         <v>1</v>
       </c>
       <c r="F91" t="s">
-        <v>992</v>
+        <v>991</v>
       </c>
       <c r="G91">
         <v>1</v>
@@ -6557,7 +6620,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="92" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:19" hidden="1" x14ac:dyDescent="0.35">
       <c r="A92" t="s">
         <v>474</v>
       </c>
@@ -6574,7 +6637,7 @@
         <v>1</v>
       </c>
       <c r="F92" t="s">
-        <v>992</v>
+        <v>991</v>
       </c>
       <c r="G92">
         <v>1</v>
@@ -6583,7 +6646,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="93" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:19" hidden="1" x14ac:dyDescent="0.35">
       <c r="A93" t="s">
         <v>477</v>
       </c>
@@ -6600,10 +6663,10 @@
         <v>1</v>
       </c>
       <c r="F93" t="s">
-        <v>992</v>
+        <v>991</v>
       </c>
       <c r="G93">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S93">
         <v>1</v>
@@ -6783,8 +6846,11 @@
       <c r="E101">
         <v>1</v>
       </c>
-      <c r="N101" t="s">
-        <v>988</v>
+      <c r="F101" t="s">
+        <v>991</v>
+      </c>
+      <c r="G101">
+        <v>1</v>
       </c>
       <c r="Q101">
         <v>1</v>
@@ -6826,8 +6892,11 @@
       <c r="E103">
         <v>1</v>
       </c>
-      <c r="N103" t="s">
-        <v>988</v>
+      <c r="F103" t="s">
+        <v>991</v>
+      </c>
+      <c r="G103">
+        <v>1</v>
       </c>
       <c r="Q103">
         <v>1</v>
@@ -7105,7 +7174,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="117" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="117" spans="1:19" hidden="1" x14ac:dyDescent="0.35">
       <c r="A117" t="s">
         <v>544</v>
       </c>
@@ -7122,10 +7191,10 @@
         <v>1</v>
       </c>
       <c r="F117" t="s">
-        <v>992</v>
+        <v>991</v>
       </c>
       <c r="G117">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q117">
         <v>1</v>
@@ -7313,11 +7382,17 @@
       <c r="E126">
         <v>1</v>
       </c>
+      <c r="F126" t="s">
+        <v>991</v>
+      </c>
+      <c r="G126">
+        <v>1</v>
+      </c>
       <c r="Q126">
         <v>1</v>
       </c>
     </row>
-    <row r="127" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="127" spans="1:19" hidden="1" x14ac:dyDescent="0.35">
       <c r="A127" t="s">
         <v>573</v>
       </c>
@@ -7334,7 +7409,7 @@
         <v>4</v>
       </c>
       <c r="G127">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q127">
         <v>1</v>
@@ -7443,7 +7518,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="133" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="133" spans="1:19" hidden="1" x14ac:dyDescent="0.35">
       <c r="A133" t="s">
         <v>589</v>
       </c>
@@ -7463,7 +7538,10 @@
         <v>4</v>
       </c>
       <c r="G133">
-        <v>1</v>
+        <v>0</v>
+      </c>
+      <c r="N133" t="s">
+        <v>1001</v>
       </c>
       <c r="Q133">
         <v>1</v>
@@ -7703,7 +7781,7 @@
         <v>1</v>
       </c>
       <c r="N145" t="s">
-        <v>990</v>
+        <v>989</v>
       </c>
       <c r="R145">
         <v>1</v>
@@ -7726,13 +7804,13 @@
         <v>1</v>
       </c>
       <c r="F146" t="s">
-        <v>992</v>
+        <v>991</v>
       </c>
       <c r="G146">
         <v>1</v>
       </c>
       <c r="N146" t="s">
-        <v>989</v>
+        <v>1002</v>
       </c>
       <c r="R146">
         <v>1</v>
@@ -8380,6 +8458,12 @@
       <c r="E178">
         <v>1</v>
       </c>
+      <c r="F178" t="s">
+        <v>991</v>
+      </c>
+      <c r="G178">
+        <v>1</v>
+      </c>
       <c r="P178">
         <v>1</v>
       </c>
@@ -8400,6 +8484,12 @@
       <c r="E179">
         <v>1</v>
       </c>
+      <c r="F179" t="s">
+        <v>991</v>
+      </c>
+      <c r="G179">
+        <v>1</v>
+      </c>
       <c r="P179">
         <v>1</v>
       </c>
@@ -8465,6 +8555,12 @@
       <c r="E183">
         <v>1</v>
       </c>
+      <c r="F183" t="s">
+        <v>991</v>
+      </c>
+      <c r="G183">
+        <v>1</v>
+      </c>
       <c r="P183">
         <v>1</v>
       </c>
@@ -8737,6 +8833,12 @@
       <c r="E199">
         <v>1</v>
       </c>
+      <c r="F199" t="s">
+        <v>991</v>
+      </c>
+      <c r="G199">
+        <v>1</v>
+      </c>
       <c r="P199">
         <v>1</v>
       </c>
@@ -8757,6 +8859,12 @@
       <c r="E200">
         <v>1</v>
       </c>
+      <c r="F200" t="s">
+        <v>991</v>
+      </c>
+      <c r="G200">
+        <v>1</v>
+      </c>
       <c r="P200">
         <v>1</v>
       </c>
@@ -8818,7 +8926,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="204" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="204" spans="1:19" hidden="1" x14ac:dyDescent="0.35">
       <c r="A204" t="s">
         <v>786</v>
       </c>
@@ -8832,7 +8940,7 @@
         <v>1</v>
       </c>
       <c r="F204" t="s">
-        <v>992</v>
+        <v>991</v>
       </c>
       <c r="G204">
         <v>1</v>
@@ -8875,7 +8983,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="207" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="207" spans="1:19" hidden="1" x14ac:dyDescent="0.35">
       <c r="A207" t="s">
         <v>793</v>
       </c>
@@ -8889,10 +8997,10 @@
         <v>1</v>
       </c>
       <c r="F207" t="s">
-        <v>992</v>
+        <v>991</v>
       </c>
       <c r="G207">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R207">
         <v>1</v>
@@ -8929,10 +9037,13 @@
         <v>1</v>
       </c>
       <c r="F209" t="s">
-        <v>992</v>
+        <v>991</v>
       </c>
       <c r="G209">
         <v>1</v>
+      </c>
+      <c r="N209" t="s">
+        <v>1005</v>
       </c>
       <c r="R209">
         <v>1</v>
@@ -8952,7 +9063,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="211" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="211" spans="1:18" hidden="1" x14ac:dyDescent="0.35">
       <c r="A211" t="s">
         <v>802</v>
       </c>
@@ -8966,16 +9077,16 @@
         <v>1</v>
       </c>
       <c r="F211" t="s">
-        <v>992</v>
+        <v>991</v>
       </c>
       <c r="G211">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R211">
         <v>1</v>
       </c>
     </row>
-    <row r="212" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="212" spans="1:18" hidden="1" x14ac:dyDescent="0.35">
       <c r="A212" t="s">
         <v>804</v>
       </c>
@@ -8989,10 +9100,10 @@
         <v>1</v>
       </c>
       <c r="F212" t="s">
-        <v>992</v>
+        <v>991</v>
       </c>
       <c r="G212">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R212">
         <v>1</v>
@@ -9012,7 +9123,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="214" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="214" spans="1:18" hidden="1" x14ac:dyDescent="0.35">
       <c r="A214" t="s">
         <v>808</v>
       </c>
@@ -9026,10 +9137,10 @@
         <v>1</v>
       </c>
       <c r="F214" t="s">
-        <v>992</v>
+        <v>991</v>
       </c>
       <c r="G214">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R214">
         <v>1</v>
@@ -9049,10 +9160,13 @@
         <v>1</v>
       </c>
       <c r="F215" t="s">
-        <v>992</v>
+        <v>991</v>
       </c>
       <c r="G215">
         <v>1</v>
+      </c>
+      <c r="N215" t="s">
+        <v>1005</v>
       </c>
       <c r="R215">
         <v>1</v>
@@ -9075,7 +9189,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="217" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="217" spans="1:18" hidden="1" x14ac:dyDescent="0.35">
       <c r="A217" t="s">
         <v>815</v>
       </c>
@@ -9092,7 +9206,7 @@
         <v>1</v>
       </c>
       <c r="F217" t="s">
-        <v>992</v>
+        <v>991</v>
       </c>
       <c r="G217">
         <v>1</v>
@@ -9155,7 +9269,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="221" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="221" spans="1:18" hidden="1" x14ac:dyDescent="0.35">
       <c r="A221" t="s">
         <v>826</v>
       </c>
@@ -9172,10 +9286,10 @@
         <v>1</v>
       </c>
       <c r="F221" t="s">
-        <v>992</v>
+        <v>991</v>
       </c>
       <c r="G221">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R221">
         <v>1</v>
@@ -9201,7 +9315,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="223" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="223" spans="1:18" hidden="1" x14ac:dyDescent="0.35">
       <c r="A223" t="s">
         <v>832</v>
       </c>
@@ -9218,7 +9332,7 @@
         <v>1</v>
       </c>
       <c r="F223" t="s">
-        <v>992</v>
+        <v>991</v>
       </c>
       <c r="G223">
         <v>1</v>
@@ -9227,7 +9341,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="224" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="224" spans="1:18" hidden="1" x14ac:dyDescent="0.35">
       <c r="A224" t="s">
         <v>835</v>
       </c>
@@ -9244,10 +9358,10 @@
         <v>1</v>
       </c>
       <c r="F224" t="s">
-        <v>992</v>
+        <v>991</v>
       </c>
       <c r="G224">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R224">
         <v>1</v>
@@ -9270,7 +9384,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="226" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="226" spans="1:18" hidden="1" x14ac:dyDescent="0.35">
       <c r="A226" t="s">
         <v>840</v>
       </c>
@@ -9287,16 +9401,16 @@
         <v>1</v>
       </c>
       <c r="F226" t="s">
-        <v>992</v>
+        <v>991</v>
       </c>
       <c r="G226">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R226">
         <v>1</v>
       </c>
     </row>
-    <row r="227" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="227" spans="1:18" hidden="1" x14ac:dyDescent="0.35">
       <c r="A227" t="s">
         <v>843</v>
       </c>
@@ -9310,7 +9424,7 @@
         <v>1</v>
       </c>
       <c r="F227" t="s">
-        <v>992</v>
+        <v>991</v>
       </c>
       <c r="G227">
         <v>1</v>
@@ -9333,7 +9447,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="229" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="229" spans="1:18" hidden="1" x14ac:dyDescent="0.35">
       <c r="A229" t="s">
         <v>847</v>
       </c>
@@ -9350,7 +9464,7 @@
         <v>4</v>
       </c>
       <c r="G229">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R229">
         <v>1</v>
@@ -9373,7 +9487,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="231" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="231" spans="1:18" hidden="1" x14ac:dyDescent="0.35">
       <c r="A231" t="s">
         <v>851</v>
       </c>
@@ -9387,7 +9501,7 @@
         <v>1</v>
       </c>
       <c r="F231" t="s">
-        <v>992</v>
+        <v>991</v>
       </c>
       <c r="G231">
         <v>1</v>
@@ -9396,7 +9510,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="232" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="232" spans="1:18" hidden="1" x14ac:dyDescent="0.35">
       <c r="A232" t="s">
         <v>853</v>
       </c>
@@ -9413,10 +9527,10 @@
         <v>1</v>
       </c>
       <c r="F232" t="s">
-        <v>992</v>
+        <v>991</v>
       </c>
       <c r="G232">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R232">
         <v>1</v>
@@ -9459,7 +9573,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="235" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="235" spans="1:18" hidden="1" x14ac:dyDescent="0.35">
       <c r="A235" t="s">
         <v>861</v>
       </c>
@@ -9476,10 +9590,10 @@
         <v>1</v>
       </c>
       <c r="F235" t="s">
-        <v>992</v>
+        <v>991</v>
       </c>
       <c r="G235">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R235">
         <v>1</v>
@@ -9522,7 +9636,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="238" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="238" spans="1:18" hidden="1" x14ac:dyDescent="0.35">
       <c r="A238" t="s">
         <v>869</v>
       </c>
@@ -9536,7 +9650,7 @@
         <v>1</v>
       </c>
       <c r="F238" t="s">
-        <v>992</v>
+        <v>991</v>
       </c>
       <c r="G238">
         <v>1</v>
@@ -9559,19 +9673,19 @@
         <v>1</v>
       </c>
       <c r="F239" t="s">
-        <v>992</v>
+        <v>991</v>
       </c>
       <c r="G239">
         <v>1</v>
       </c>
       <c r="N239" t="s">
-        <v>991</v>
+        <v>990</v>
       </c>
       <c r="R239">
         <v>1</v>
       </c>
     </row>
-    <row r="240" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="240" spans="1:18" hidden="1" x14ac:dyDescent="0.35">
       <c r="A240" t="s">
         <v>873</v>
       </c>
@@ -9588,10 +9702,10 @@
         <v>1</v>
       </c>
       <c r="F240" t="s">
-        <v>992</v>
+        <v>991</v>
       </c>
       <c r="G240">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R240">
         <v>1</v>
@@ -9631,7 +9745,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="243" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="243" spans="1:19" hidden="1" x14ac:dyDescent="0.35">
       <c r="A243" t="s">
         <v>882</v>
       </c>
@@ -9648,13 +9762,13 @@
         <v>4</v>
       </c>
       <c r="G243">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S243">
         <v>1</v>
       </c>
     </row>
-    <row r="244" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="244" spans="1:19" hidden="1" x14ac:dyDescent="0.35">
       <c r="A244" t="s">
         <v>884</v>
       </c>
@@ -9668,16 +9782,16 @@
         <v>1</v>
       </c>
       <c r="F244" t="s">
-        <v>992</v>
+        <v>991</v>
       </c>
       <c r="G244">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R244">
         <v>1</v>
       </c>
     </row>
-    <row r="245" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="245" spans="1:19" hidden="1" x14ac:dyDescent="0.35">
       <c r="A245" t="s">
         <v>886</v>
       </c>
@@ -9691,7 +9805,7 @@
         <v>1</v>
       </c>
       <c r="F245" t="s">
-        <v>992</v>
+        <v>991</v>
       </c>
       <c r="G245">
         <v>1</v>
@@ -9700,7 +9814,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="246" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="246" spans="1:19" hidden="1" x14ac:dyDescent="0.35">
       <c r="A246" t="s">
         <v>887</v>
       </c>
@@ -9714,7 +9828,7 @@
         <v>1</v>
       </c>
       <c r="F246" t="s">
-        <v>992</v>
+        <v>991</v>
       </c>
       <c r="G246">
         <v>1</v>
@@ -9723,7 +9837,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="247" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="247" spans="1:19" hidden="1" x14ac:dyDescent="0.35">
       <c r="A247" t="s">
         <v>889</v>
       </c>
@@ -9740,7 +9854,7 @@
         <v>1</v>
       </c>
       <c r="F247" t="s">
-        <v>992</v>
+        <v>991</v>
       </c>
       <c r="G247">
         <v>1</v>
@@ -9749,7 +9863,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="248" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="248" spans="1:19" hidden="1" x14ac:dyDescent="0.35">
       <c r="A248" t="s">
         <v>892</v>
       </c>
@@ -9766,7 +9880,7 @@
         <v>1</v>
       </c>
       <c r="F248" t="s">
-        <v>992</v>
+        <v>991</v>
       </c>
       <c r="G248">
         <v>1</v>
@@ -9775,7 +9889,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="249" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="249" spans="1:19" hidden="1" x14ac:dyDescent="0.35">
       <c r="A249" t="s">
         <v>895</v>
       </c>
@@ -9792,7 +9906,7 @@
         <v>1</v>
       </c>
       <c r="F249" t="s">
-        <v>992</v>
+        <v>991</v>
       </c>
       <c r="G249">
         <v>1</v>
@@ -9801,7 +9915,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="250" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="250" spans="1:19" hidden="1" x14ac:dyDescent="0.35">
       <c r="A250" t="s">
         <v>898</v>
       </c>
@@ -9815,16 +9929,16 @@
         <v>1</v>
       </c>
       <c r="F250" t="s">
-        <v>992</v>
+        <v>991</v>
       </c>
       <c r="G250">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O250">
         <v>1</v>
       </c>
     </row>
-    <row r="251" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="251" spans="1:19" hidden="1" x14ac:dyDescent="0.35">
       <c r="A251" t="s">
         <v>900</v>
       </c>
@@ -9838,13 +9952,16 @@
         <v>1</v>
       </c>
       <c r="F251" t="s">
-        <v>992</v>
+        <v>991</v>
       </c>
       <c r="G251">
         <v>1</v>
       </c>
-    </row>
-    <row r="252" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="S251">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="252" spans="1:19" hidden="1" x14ac:dyDescent="0.35">
       <c r="A252" t="s">
         <v>902</v>
       </c>
@@ -9861,10 +9978,10 @@
         <v>1</v>
       </c>
       <c r="F252" t="s">
-        <v>992</v>
+        <v>991</v>
       </c>
       <c r="G252">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O252">
         <v>1</v>
@@ -9884,10 +10001,13 @@
         <v>1</v>
       </c>
       <c r="F253" t="s">
-        <v>992</v>
+        <v>991</v>
       </c>
       <c r="G253">
         <v>1</v>
+      </c>
+      <c r="N253" t="s">
+        <v>1003</v>
       </c>
       <c r="O253">
         <v>1</v>
@@ -9924,10 +10044,13 @@
         <v>1</v>
       </c>
       <c r="F255" t="s">
-        <v>992</v>
+        <v>991</v>
       </c>
       <c r="G255">
         <v>1</v>
+      </c>
+      <c r="N255" t="s">
+        <v>1006</v>
       </c>
       <c r="Q255">
         <v>1</v>
@@ -10001,7 +10124,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="260" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="260" spans="1:19" hidden="1" x14ac:dyDescent="0.35">
       <c r="A260" t="s">
         <v>921</v>
       </c>
@@ -10015,7 +10138,7 @@
         <v>1</v>
       </c>
       <c r="F260" t="s">
-        <v>992</v>
+        <v>991</v>
       </c>
       <c r="G260">
         <v>1</v>
@@ -10024,12 +10147,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="261" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="261" spans="1:19" hidden="1" x14ac:dyDescent="0.35">
       <c r="A261" t="s">
+        <v>993</v>
+      </c>
+      <c r="B261" t="s">
         <v>994</v>
-      </c>
-      <c r="B261" t="s">
-        <v>995</v>
       </c>
       <c r="D261">
         <v>1</v>
@@ -10041,13 +10164,13 @@
         <v>4</v>
       </c>
       <c r="G261">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q261">
         <v>1</v>
       </c>
     </row>
-    <row r="262" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="262" spans="1:19" hidden="1" x14ac:dyDescent="0.35">
       <c r="A262" t="s">
         <v>923</v>
       </c>
@@ -10096,7 +10219,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="264" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="264" spans="1:19" hidden="1" x14ac:dyDescent="0.35">
       <c r="A264" t="s">
         <v>929</v>
       </c>
@@ -10113,7 +10236,7 @@
         <v>1</v>
       </c>
       <c r="F264" t="s">
-        <v>992</v>
+        <v>991</v>
       </c>
       <c r="G264">
         <v>1</v>
@@ -10145,7 +10268,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="266" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="266" spans="1:19" hidden="1" x14ac:dyDescent="0.35">
       <c r="A266" t="s">
         <v>935</v>
       </c>
@@ -10162,10 +10285,10 @@
         <v>1</v>
       </c>
       <c r="F266" t="s">
-        <v>992</v>
+        <v>991</v>
       </c>
       <c r="G266">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R266">
         <v>1</v>
@@ -10185,10 +10308,13 @@
         <v>1</v>
       </c>
       <c r="F267" t="s">
-        <v>992</v>
+        <v>991</v>
       </c>
       <c r="G267">
         <v>1</v>
+      </c>
+      <c r="N267" t="s">
+        <v>1007</v>
       </c>
       <c r="R267">
         <v>1</v>
@@ -10214,7 +10340,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="269" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="269" spans="1:19" hidden="1" x14ac:dyDescent="0.35">
       <c r="A269" t="s">
         <v>942</v>
       </c>
@@ -10231,16 +10357,16 @@
         <v>1</v>
       </c>
       <c r="F269" t="s">
-        <v>992</v>
+        <v>991</v>
       </c>
       <c r="G269">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R269">
         <v>1</v>
       </c>
     </row>
-    <row r="270" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="270" spans="1:19" hidden="1" x14ac:dyDescent="0.35">
       <c r="A270" t="s">
         <v>944</v>
       </c>
@@ -10260,7 +10386,7 @@
         <v>4</v>
       </c>
       <c r="G270">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R270">
         <v>1</v>
@@ -10289,7 +10415,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="272" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="272" spans="1:19" hidden="1" x14ac:dyDescent="0.35">
       <c r="A272" t="s">
         <v>948</v>
       </c>
@@ -10306,7 +10432,7 @@
         <v>1</v>
       </c>
       <c r="F272" t="s">
-        <v>992</v>
+        <v>991</v>
       </c>
       <c r="G272">
         <v>1</v>
@@ -10315,7 +10441,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="273" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="273" spans="1:19" hidden="1" x14ac:dyDescent="0.35">
       <c r="A273" t="s">
         <v>950</v>
       </c>
@@ -10332,7 +10458,7 @@
         <v>1</v>
       </c>
       <c r="F273" t="s">
-        <v>992</v>
+        <v>991</v>
       </c>
       <c r="G273">
         <v>1</v>
@@ -10341,7 +10467,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="274" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="274" spans="1:19" hidden="1" x14ac:dyDescent="0.35">
       <c r="A274" t="s">
         <v>952</v>
       </c>
@@ -10358,16 +10484,16 @@
         <v>1</v>
       </c>
       <c r="F274" t="s">
-        <v>992</v>
+        <v>991</v>
       </c>
       <c r="G274">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S274">
         <v>1</v>
       </c>
     </row>
-    <row r="275" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="275" spans="1:19" hidden="1" x14ac:dyDescent="0.35">
       <c r="A275" t="s">
         <v>955</v>
       </c>
@@ -10384,10 +10510,10 @@
         <v>1</v>
       </c>
       <c r="F275" t="s">
-        <v>992</v>
+        <v>991</v>
       </c>
       <c r="G275">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S275">
         <v>1</v>
@@ -10407,7 +10533,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="277" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="277" spans="1:19" hidden="1" x14ac:dyDescent="0.35">
       <c r="A277" t="s">
         <v>960</v>
       </c>
@@ -10424,10 +10550,10 @@
         <v>1</v>
       </c>
       <c r="F277" t="s">
-        <v>992</v>
+        <v>991</v>
       </c>
       <c r="G277">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R277">
         <v>1</v>
@@ -10493,7 +10619,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="281" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="281" spans="1:19" hidden="1" x14ac:dyDescent="0.35">
       <c r="A281" t="s">
         <v>971</v>
       </c>
@@ -10510,7 +10636,7 @@
         <v>1</v>
       </c>
       <c r="F281" t="s">
-        <v>992</v>
+        <v>991</v>
       </c>
       <c r="G281">
         <v>1</v>
@@ -10536,7 +10662,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="283" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="283" spans="1:19" hidden="1" x14ac:dyDescent="0.35">
       <c r="A283" t="s">
         <v>977</v>
       </c>
@@ -10556,13 +10682,13 @@
         <v>4</v>
       </c>
       <c r="G283">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O283">
         <v>1</v>
       </c>
     </row>
-    <row r="284" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="284" spans="1:19" hidden="1" x14ac:dyDescent="0.35">
       <c r="A284" t="s">
         <v>982</v>
       </c>
@@ -10579,20 +10705,23 @@
         <v>1</v>
       </c>
       <c r="F284" t="s">
-        <v>992</v>
+        <v>991</v>
       </c>
       <c r="G284">
+        <v>1</v>
+      </c>
+      <c r="S284">
         <v>1</v>
       </c>
     </row>
   </sheetData>
   <autoFilter ref="A1:T284" xr:uid="{00000000-0001-0000-0200-000000000000}">
-    <filterColumn colId="4">
-      <customFilters>
-        <customFilter operator="notEqual" val=" "/>
-      </customFilters>
+    <filterColumn colId="6">
+      <filters>
+        <filter val="1"/>
+      </filters>
     </filterColumn>
-    <filterColumn colId="5">
+    <filterColumn colId="13">
       <customFilters>
         <customFilter operator="notEqual" val=" "/>
       </customFilters>

</xml_diff>